<commit_message>
GMT fix, html e-mail improved
</commit_message>
<xml_diff>
--- a/busca.xlsx
+++ b/busca.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\Web-scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD76022-2685-400C-81F1-4760A1EE9233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315DC1CE-244E-484A-BDE0-23B2AD00D679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10710" yWindow="0" windowWidth="25935" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +483,6 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -664,9 +663,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{32EFFF0B-6FB1-4751-B765-4DEAFEE49783}"/>
-    <hyperlink ref="I3" r:id="rId2" xr:uid="{58FECB2D-39E4-4FFE-94CA-7A7795D251E4}"/>
-    <hyperlink ref="I4:I8" r:id="rId3" display="tuliovfarias@gmail.com" xr:uid="{E0E0B873-22F4-4A9F-9821-7A7FE5FF8D8E}"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{D01F376F-F2E7-461D-8434-C1F5E490F904}"/>
+    <hyperlink ref="I3" r:id="rId2" xr:uid="{CEC1CC7D-10DC-4BED-984D-3D528C6A48AA}"/>
+    <hyperlink ref="I4:I8" r:id="rId3" display="tuliovfarias@gmail.com" xr:uid="{63716191-E705-4190-BABF-A2CA86AD8788}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>

</xml_diff>